<commit_message>
cabeceras de archivo ok
</commit_message>
<xml_diff>
--- a/parametrizaion.xlsx
+++ b/parametrizaion.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Categorias" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="121">
   <si>
     <t xml:space="preserve">CODIGO</t>
   </si>
@@ -34,81 +34,102 @@
     <t xml:space="preserve">Posición</t>
   </si>
   <si>
+    <t xml:space="preserve">Nombre Categoria</t>
+  </si>
+  <si>
     <t xml:space="preserve">1001</t>
   </si>
   <si>
     <t xml:space="preserve">16</t>
   </si>
   <si>
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Categoriatest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3031</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Categoria2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3033</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Categoria3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3121</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Categoria4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3125</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Categoria5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Categoria6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CodigoCategoria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Codigo de Columna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nombre Campo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es campo Multivalor?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es Etiqueta?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relación con el Campo Etiqueta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presenta?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuenta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moneda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FieldName1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FieldName2</t>
+  </si>
+  <si>
     <t xml:space="preserve">5</t>
   </si>
   <si>
-    <t xml:space="preserve">3031</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3033</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3121</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3125</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CodigoCategoria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Codigo de Columna</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nombre Campo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Es campo Multivalor?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Es Etiqueta?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Relación con el Campo Etiqueta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Presenta?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cuenta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moneda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FieldName1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FieldName2</t>
-  </si>
-  <si>
     <t xml:space="preserve">FieldValue1</t>
   </si>
   <si>
@@ -184,7 +205,7 @@
     <t xml:space="preserve">Código Columna</t>
   </si>
   <si>
-    <t xml:space="preserve">Código Campo Etiqueta</t>
+    <t xml:space="preserve">Código Campo Subcampo</t>
   </si>
   <si>
     <t xml:space="preserve">Orden de Sub Campo</t>
@@ -375,7 +396,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -400,6 +421,14 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -468,7 +497,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -489,7 +518,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -507,10 +536,6 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -534,14 +559,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -622,17 +639,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1048576"/>
+  <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="10.49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -645,71 +664,92 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>4</v>
-      </c>
       <c r="C4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>4</v>
-      </c>
       <c r="C5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>4</v>
-      </c>
       <c r="C6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>5</v>
+      <c r="C7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -735,14 +775,14 @@
   </sheetPr>
   <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.49"/>
@@ -752,747 +792,747 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F2" s="4"/>
-      <c r="G2" s="5" t="s">
-        <v>21</v>
+      <c r="G2" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F3" s="4"/>
-      <c r="G3" s="5" t="s">
-        <v>21</v>
+      <c r="G3" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="F4" s="4"/>
-      <c r="G4" s="5" t="s">
-        <v>21</v>
+      <c r="G4" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="F5" s="4"/>
-      <c r="G5" s="5" t="s">
-        <v>21</v>
+      <c r="G5" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F6" s="4"/>
-      <c r="G6" s="5" t="s">
-        <v>21</v>
+      <c r="G6" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>21</v>
+        <v>31</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F9" s="4"/>
-      <c r="G9" s="5" t="s">
-        <v>21</v>
+      <c r="G9" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F10" s="4"/>
-      <c r="G10" s="5" t="s">
-        <v>21</v>
+      <c r="G10" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F11" s="4"/>
-      <c r="G11" s="5" t="s">
-        <v>21</v>
+      <c r="G11" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F12" s="4"/>
-      <c r="G12" s="5" t="s">
-        <v>21</v>
+      <c r="G12" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F13" s="4"/>
-      <c r="G13" s="5" t="s">
-        <v>21</v>
+      <c r="G13" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F14" s="4"/>
-      <c r="G14" s="5" t="s">
-        <v>21</v>
+      <c r="G14" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F15" s="4"/>
-      <c r="G15" s="5" t="s">
-        <v>20</v>
+      <c r="G15" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F16" s="4"/>
-      <c r="G16" s="5" t="s">
-        <v>21</v>
+      <c r="G16" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F17" s="4"/>
-      <c r="G17" s="5" t="s">
-        <v>21</v>
+      <c r="G17" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F18" s="4"/>
-      <c r="G18" s="5" t="s">
-        <v>21</v>
+      <c r="G18" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F19" s="4"/>
-      <c r="G19" s="5" t="s">
-        <v>21</v>
+      <c r="G19" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F20" s="4"/>
-      <c r="G20" s="5" t="s">
-        <v>21</v>
+      <c r="G20" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="16.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="F21" s="4"/>
-      <c r="G21" s="5" t="s">
-        <v>21</v>
+      <c r="G21" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="F22" s="4"/>
-      <c r="G22" s="5" t="s">
-        <v>21</v>
+      <c r="G22" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F23" s="4"/>
-      <c r="G23" s="5" t="s">
-        <v>21</v>
+      <c r="G23" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>21</v>
+        <v>31</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F26" s="4"/>
-      <c r="G26" s="5" t="s">
-        <v>21</v>
+      <c r="G26" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F27" s="4"/>
-      <c r="G27" s="5" t="s">
-        <v>21</v>
+      <c r="G27" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F28" s="4"/>
-      <c r="G28" s="5" t="s">
-        <v>21</v>
+      <c r="G28" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F29" s="4"/>
-      <c r="G29" s="5" t="s">
-        <v>21</v>
+      <c r="G29" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F30" s="4"/>
-      <c r="G30" s="5" t="s">
-        <v>21</v>
+      <c r="G30" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F31" s="4"/>
-      <c r="G31" s="5" t="s">
-        <v>21</v>
+      <c r="G31" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F32" s="4"/>
-      <c r="G32" s="5" t="s">
-        <v>20</v>
+      <c r="G32" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F33" s="4"/>
-      <c r="G33" s="5" t="s">
-        <v>21</v>
+      <c r="G33" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F34" s="4"/>
-      <c r="G34" s="5" t="s">
-        <v>21</v>
+      <c r="G34" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F35" s="4"/>
-      <c r="G35" s="5" t="s">
-        <v>21</v>
+      <c r="G35" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1514,16 +1554,16 @@
   </sheetPr>
   <dimension ref="A2:G14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="10.49"/>
@@ -1531,264 +1571,264 @@
   <sheetData>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="E4" s="8" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>24</v>
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>24</v>
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="E9" s="8" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>26</v>
+        <v>4</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>26</v>
+        <v>16</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>20</v>
+        <v>25</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>31</v>
+        <v>16</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>20</v>
+        <v>29</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="12"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="11"/>
       <c r="E13" s="8"/>
-      <c r="F13" s="10"/>
+      <c r="F13" s="8"/>
       <c r="G13" s="8"/>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1797,7 +1837,7 @@
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
-      <c r="F14" s="10"/>
+      <c r="F14" s="8"/>
       <c r="G14" s="8"/>
     </row>
   </sheetData>
@@ -1824,7 +1864,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="68.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="68.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="4" style="0" width="10.49"/>
@@ -1836,222 +1876,222 @@
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="14" t="s">
-        <v>63</v>
+      <c r="A3" s="13" t="s">
+        <v>70</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="N3" s="3"/>
       <c r="O3" s="3" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" s="3" customFormat="true" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="H4" s="15" t="s">
+      <c r="A4" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="J4" s="15" t="s">
+      <c r="C4" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="K4" s="15" t="s">
+      <c r="D4" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="L4" s="15"/>
+      <c r="E4" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="K4" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="L4" s="14"/>
     </row>
     <row r="5" s="3" customFormat="true" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="14" t="s">
-        <v>89</v>
+      <c r="A5" s="13" t="s">
+        <v>96</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" s="3" customFormat="true" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="14" t="s">
-        <v>66</v>
+      <c r="A6" s="13" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="7" s="3" customFormat="true" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="14" t="s">
-        <v>100</v>
+      <c r="A7" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" s="3" customFormat="true" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="14"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="3" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" s="3" customFormat="true" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="14"/>
+      <c r="A9" s="13"/>
     </row>
     <row r="10" s="3" customFormat="true" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="14"/>
+      <c r="A10" s="13"/>
     </row>
     <row r="11" s="3" customFormat="true" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="14"/>
+      <c r="A11" s="13"/>
     </row>
     <row r="12" s="3" customFormat="true" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="14"/>
+      <c r="A12" s="13"/>
     </row>
     <row r="13" s="3" customFormat="true" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>110</v>
+      <c r="A13" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>117</v>
       </c>
       <c r="F13" s="0"/>
       <c r="G13" s="0"/>
@@ -2081,105 +2121,105 @@
       </c>
     </row>
     <row r="14" s="3" customFormat="true" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="14" t="s">
-        <v>64</v>
+      <c r="A14" s="13" t="s">
+        <v>71</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D14" s="14" t="str">
+        <v>70</v>
+      </c>
+      <c r="D14" s="13" t="str">
         <f aca="false">A14</f>
         <v>PEN</v>
       </c>
-      <c r="E14" s="17" t="str">
+      <c r="E14" s="12" t="str">
         <f aca="false">A31</f>
         <v>TOTCOMMITMENT</v>
       </c>
-      <c r="F14" s="17" t="str">
+      <c r="F14" s="12" t="str">
         <f aca="false">A32</f>
         <v>CURCOMMITMENT</v>
       </c>
-      <c r="G14" s="17" t="str">
+      <c r="G14" s="12" t="str">
         <f aca="false">A33</f>
         <v>TOTCOMMITMENTBL</v>
       </c>
-      <c r="H14" s="17" t="str">
+      <c r="H14" s="12" t="str">
         <f aca="false">A34</f>
         <v>CURCOMMITMENTBL</v>
       </c>
-      <c r="I14" s="14" t="str">
+      <c r="I14" s="13" t="str">
         <f aca="false">A35</f>
         <v>AVLACCOUNT</v>
       </c>
-      <c r="J14" s="14" t="str">
+      <c r="J14" s="13" t="str">
         <f aca="false">A36</f>
         <v>AVLACCOUNTBL</v>
       </c>
-      <c r="K14" s="14" t="str">
+      <c r="K14" s="13" t="str">
         <f aca="false">A37</f>
         <v>CURACCOUNT</v>
       </c>
-      <c r="L14" s="14" t="str">
+      <c r="L14" s="13" t="str">
         <f aca="false">A38</f>
         <v>DUECLINSURANCE</v>
       </c>
-      <c r="M14" s="14" t="str">
+      <c r="M14" s="13" t="str">
         <f aca="false">A39</f>
         <v>DUEPENALTY3D</v>
       </c>
-      <c r="N14" s="14" t="str">
+      <c r="N14" s="13" t="str">
         <f aca="false">A40</f>
         <v>DUEACCOUNT</v>
       </c>
-      <c r="O14" s="14" t="str">
+      <c r="O14" s="13" t="str">
         <f aca="false">A41</f>
         <v>DUEPRINCIPALINT</v>
       </c>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
+      <c r="P14" s="0"/>
+      <c r="Q14" s="0"/>
     </row>
     <row r="15" s="3" customFormat="true" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="14" t="s">
-        <v>111</v>
+      <c r="A15" s="13" t="s">
+        <v>118</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D15" s="14" t="str">
+        <v>70</v>
+      </c>
+      <c r="D15" s="13" t="str">
         <f aca="false">A15</f>
         <v>TOTCOMMITMENT]CURCOMMITMENT]TOTCOMMITMENTBL]CURCOMMITMENTBL]AVLACCOUNT]AVLACCOUNTBL]CURACCOUNT]DUECLINSURANCE]DUEPENALTY3D]DUEACCOUNT]DUEPRINCIPALINT</v>
       </c>
-      <c r="E15" s="14" t="str">
+      <c r="E15" s="13" t="str">
         <f aca="false">A44</f>
         <v>-4290</v>
       </c>
-      <c r="F15" s="14" t="str">
+      <c r="F15" s="13" t="str">
         <f aca="false">A45</f>
         <v>-4290</v>
       </c>
-      <c r="G15" s="14" t="n">
+      <c r="G15" s="13" t="n">
         <f aca="false">A46</f>
         <v>0</v>
       </c>
-      <c r="H15" s="17" t="str">
+      <c r="H15" s="12" t="str">
         <f aca="false">A48</f>
         <v>-4290</v>
       </c>
-      <c r="I15" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="J15" s="14" t="str">
+      <c r="I15" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="J15" s="13" t="str">
         <f aca="false">A50</f>
         <v>-4290</v>
       </c>
-      <c r="K15" s="14" t="str">
+      <c r="K15" s="13" t="str">
         <f aca="false">A51</f>
         <v>-139.96</v>
       </c>
-      <c r="L15" s="14" t="str">
+      <c r="L15" s="13" t="str">
         <f aca="false">A52</f>
         <v>-1400</v>
       </c>
@@ -2191,50 +2231,50 @@
         <f aca="false">A54</f>
         <v>-1654.22</v>
       </c>
-      <c r="O15" s="18" t="n">
+      <c r="O15" s="0" t="n">
         <f aca="false">A55</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" s="3" customFormat="true" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="14" t="s">
-        <v>65</v>
+      <c r="A16" s="13" t="s">
+        <v>72</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D16" s="14" t="str">
+        <v>70</v>
+      </c>
+      <c r="D16" s="13" t="str">
         <f aca="false">A16</f>
         <v>TOTCOMMITMENT-20200430]CURCOMMITMENT-20200430]TOTCOMMITMENTBL-20200430]CURCOMMITMENTBL-20200430]AVLACCOUNT-20200430]AVLACCOUNTBL-20200430]CURACCOUNT-20200430]DUECLINSURANCE-20200430]DUEPENALTY3D-20200430]DUEACCOUNT-20200430]DUEPRINCIPALINT-20200430</v>
       </c>
-      <c r="E16" s="14" t="str">
+      <c r="E16" s="13" t="str">
         <f aca="false">A45</f>
         <v>-4290</v>
       </c>
-      <c r="F16" s="14" t="n">
+      <c r="F16" s="13" t="n">
         <f aca="false">A46</f>
         <v>0</v>
       </c>
-      <c r="G16" s="14" t="str">
+      <c r="G16" s="13" t="str">
         <f aca="false">A47</f>
         <v>-4290</v>
       </c>
-      <c r="H16" s="17" t="str">
+      <c r="H16" s="12" t="str">
         <f aca="false">A49</f>
         <v>-4290</v>
       </c>
-      <c r="I16" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="J16" s="14" t="str">
+      <c r="I16" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="J16" s="13" t="str">
         <f aca="false">A51</f>
         <v>-139.96</v>
       </c>
-      <c r="K16" s="14" t="str">
+      <c r="K16" s="13" t="str">
         <f aca="false">A52</f>
         <v>-1400</v>
       </c>
-      <c r="L16" s="14" t="str">
+      <c r="L16" s="13" t="str">
         <f aca="false">A53</f>
         <v>-7394.8</v>
       </c>
@@ -2246,168 +2286,168 @@
         <f aca="false">A55</f>
         <v>0</v>
       </c>
-      <c r="O16" s="18" t="n">
+      <c r="O16" s="0" t="n">
         <f aca="false">A56</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" s="3" customFormat="true" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="14" t="s">
-        <v>66</v>
+      <c r="A17" s="13" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="18" s="3" customFormat="true" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="14" t="s">
-        <v>67</v>
+      <c r="A18" s="13" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="19" s="3" customFormat="true" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="14" t="s">
-        <v>68</v>
+      <c r="A19" s="13" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="20" s="3" customFormat="true" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="14" t="s">
-        <v>69</v>
+      <c r="A20" s="13" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="21" s="3" customFormat="true" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="E21" s="16" t="s">
-        <v>110</v>
+      <c r="A21" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>117</v>
       </c>
       <c r="F21" s="0"/>
       <c r="G21" s="0"/>
       <c r="H21" s="0"/>
       <c r="I21" s="0"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
     </row>
     <row r="22" s="3" customFormat="true" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="G22" s="15" t="s">
+      <c r="A22" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="H22" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="I22" s="13"/>
+    </row>
+    <row r="23" s="3" customFormat="true" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="H22" s="15" t="s">
+    </row>
+    <row r="24" s="3" customFormat="true" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="I22" s="14"/>
-    </row>
-    <row r="23" s="3" customFormat="true" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="14" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="24" s="3" customFormat="true" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="14" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="25" s="3" customFormat="true" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="14" t="s">
-        <v>74</v>
+      <c r="A25" s="13" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="26" s="3" customFormat="true" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="14" t="s">
-        <v>74</v>
+      <c r="A26" s="13" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="14" t="s">
-        <v>75</v>
+      <c r="A27" s="13" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="14" t="s">
-        <v>76</v>
+      <c r="A28" s="13" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="14" t="s">
-        <v>77</v>
+      <c r="A29" s="13" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="15" t="s">
-        <v>78</v>
+      <c r="A31" s="14" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="15" t="s">
-        <v>79</v>
+      <c r="A32" s="14" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="15" t="s">
-        <v>80</v>
+      <c r="A33" s="14" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="15" t="s">
-        <v>81</v>
+      <c r="A34" s="14" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="15" t="s">
-        <v>82</v>
+      <c r="A35" s="14" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="15" t="s">
-        <v>83</v>
+      <c r="A36" s="14" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="15" t="s">
-        <v>84</v>
+      <c r="A37" s="14" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="15" t="s">
-        <v>85</v>
+      <c r="A38" s="14" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="15" t="s">
-        <v>86</v>
+      <c r="A39" s="14" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="15" t="s">
-        <v>87</v>
+      <c r="A40" s="14" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="15" t="s">
-        <v>88</v>
+      <c r="A41" s="14" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="15"/>
+      <c r="A42" s="14"/>
     </row>
     <row r="44" customFormat="false" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="14" t="s">
-        <v>100</v>
+      <c r="A44" s="13" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2415,42 +2455,42 @@
     </row>
     <row r="47" customFormat="false" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="3" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="3" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="3" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="11.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>